<commit_message>
Weigh-in Form: Highlight minors
</commit_message>
<xml_diff>
--- a/local/templates/weighin/WeighInForm.xlsx
+++ b/local/templates/weighin/WeighInForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/usaw-owlcms/local/templates/weighin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE13CD6-C8FE-C14C-A54B-3EE52A33954A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23236522-88C7-8E49-A4C3-C802199A1981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="500" windowWidth="39500" windowHeight="23500" xr2:uid="{295DEE46-55CB-FD4C-B22D-54961E31048E}"/>
+    <workbookView xWindow="20520" yWindow="2600" windowWidth="39500" windowHeight="23500" xr2:uid="{295DEE46-55CB-FD4C-B22D-54961E31048E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -483,13 +483,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -854,21 +891,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -1068,6 +1105,11 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="B9:G9"/>
   </mergeCells>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="greaterThan">
+      <formula>DATE(YEAR(A4) - 18, MONTH(A4), DAY(A4))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -1100,21 +1142,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -1315,7 +1357,7 @@
     <mergeCell ref="I9:M9"/>
   </mergeCells>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>DATEDIF(F7, $A$4, "Y") &lt; 18</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>